<commit_message>
[Common] Update email, formula
Description:
  - <desc>

Affected files:
  - <files>
</commit_message>
<xml_diff>
--- a/build/MarketCollect/data/Check-Price-AMZ-EBAY.xlsx
+++ b/build/MarketCollect/data/Check-Price-AMZ-EBAY.xlsx
@@ -11,14 +11,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$L$49</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="15">
+  <fonts count="11">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -48,12 +48,6 @@
     </font>
     <font>
       <name val="Arial"/>
-      <color rgb="FF0000FF"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <b val="1"/>
       <color theme="1"/>
       <sz val="10"/>
@@ -62,24 +56,6 @@
       <name val="Roboto"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color rgb="FF1155CC"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color rgb="FFE4AF09"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color rgb="FFE4AF09"/>
-      <sz val="10"/>
-      <u val="single"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -156,10 +132,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -168,7 +144,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -179,46 +155,31 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -227,19 +188,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -526,22 +475,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col width="7.28515625" customWidth="1" style="16" min="1" max="1"/>
-    <col width="35.85546875" customWidth="1" style="16" min="2" max="2"/>
-    <col width="26.85546875" customWidth="1" style="16" min="3" max="3"/>
-    <col width="16.28515625" customWidth="1" style="16" min="4" max="4"/>
-    <col width="24.5703125" customWidth="1" style="16" min="5" max="5"/>
-    <col width="20" customWidth="1" style="16" min="6" max="6"/>
-    <col width="23.42578125" customWidth="1" style="16" min="7" max="7"/>
-    <col width="32.140625" customWidth="1" style="16" min="8" max="8"/>
-    <col width="22.7109375" customWidth="1" style="17" min="9" max="9"/>
-    <col width="17.7109375" customWidth="1" style="18" min="10" max="10"/>
-    <col width="18.42578125" customWidth="1" style="16" min="11" max="11"/>
+    <col width="7.28515625" customWidth="1" style="14" min="1" max="1"/>
+    <col width="35.85546875" customWidth="1" style="14" min="2" max="2"/>
+    <col width="26.85546875" customWidth="1" style="14" min="3" max="3"/>
+    <col width="16.28515625" customWidth="1" style="14" min="4" max="4"/>
+    <col width="24.5703125" customWidth="1" style="14" min="5" max="5"/>
+    <col width="20" customWidth="1" style="14" min="6" max="6"/>
+    <col width="23.42578125" customWidth="1" style="14" min="7" max="7"/>
+    <col width="32.140625" customWidth="1" style="14" min="8" max="8"/>
+    <col width="22.7109375" customWidth="1" style="15" min="9" max="9"/>
+    <col width="17.7109375" customWidth="1" style="16" min="10" max="10"/>
+    <col width="18.42578125" customWidth="1" style="14" min="11" max="11"/>
     <col width="19.85546875" customWidth="1" style="5" min="12" max="12"/>
     <col width="22.85546875" customWidth="1" style="5" min="16" max="19"/>
   </cols>
@@ -609,15 +558,15 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" s="5">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="inlineStr">
+      <c r="B2" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174539584685</t>
         </is>
       </c>
-      <c r="C2" s="25" t="inlineStr">
+      <c r="C2" s="19" t="inlineStr">
         <is>
           <t>5/16" 4 Stud Power Distribution Block BUSBAR With Cover, Stainless Steel(Black)</t>
         </is>
@@ -627,7 +576,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E2" s="16" t="inlineStr">
+      <c r="E2" s="14" t="inlineStr">
         <is>
           <t>35.99</t>
         </is>
@@ -637,26 +586,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G2" s="22" t="inlineStr">
+      <c r="G2" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B07C5SBZ4M/ref=sspa_dk_detail_0?pd_rd_i=B07CCGCWKD&amp;amp;th=1</t>
         </is>
       </c>
-      <c r="H2" s="24" t="inlineStr">
+      <c r="H2" s="19" t="inlineStr">
         <is>
           <t>(Black) 5/16" 4 Stud Power Distribution Block -BUSBAR- with Cover</t>
         </is>
       </c>
-      <c r="I2" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J2" s="18" t="n">
+      <c r="I2" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J2" s="16" t="n">
         <v>19.99</v>
       </c>
-      <c r="K2" s="14">
-        <f>A2+B2+AC1</f>
+      <c r="K2" s="13">
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L2" s="3" t="n"/>
@@ -671,15 +620,15 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" s="5">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="inlineStr">
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174567073351</t>
         </is>
       </c>
-      <c r="C3" s="25" t="inlineStr">
+      <c r="C3" s="19" t="inlineStr">
         <is>
           <t>Aluminum Deer Cart Transport Gear Haul Folds Flat Hunting Outdoor Sport Haul New</t>
         </is>
@@ -689,7 +638,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E3" s="16" t="inlineStr">
+      <c r="E3" s="14" t="inlineStr">
         <is>
           <t>109.99</t>
         </is>
@@ -699,26 +648,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G3" s="22" t="inlineStr">
+      <c r="G3" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/Goplus-Folding-Capacity-Utility-Accessories/dp/B01HI69CB6/</t>
         </is>
       </c>
-      <c r="H3" s="24" t="inlineStr">
+      <c r="H3" s="19" t="inlineStr">
         <is>
           <t>Goplus Folding Deer Game Cart Larger Capacity 500lbs Hauler Utility Gear Dolly Cart Hunting Accessories</t>
         </is>
       </c>
-      <c r="I3" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J3" s="18" t="n">
+      <c r="I3" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J3" s="16" t="n">
         <v>85.98999999999999</v>
       </c>
       <c r="K3">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L3" s="3" t="n"/>
@@ -733,25 +682,25 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" s="5">
-      <c r="A4" s="14" t="n">
+      <c r="A4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="inlineStr">
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>https://www.ebay.com/itm/174532088103</t>
         </is>
       </c>
-      <c r="C4" s="26" t="inlineStr">
+      <c r="C4" s="19" t="inlineStr">
         <is>
           <t>Baby Safety Gate Door Walk Through Pet Indoor Dog Fence Lock Extra Wide Tall New</t>
         </is>
       </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E4" s="16" t="inlineStr">
+      <c r="D4" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E4" s="14" t="inlineStr">
         <is>
           <t>51.99</t>
         </is>
@@ -761,26 +710,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G4" s="22" t="inlineStr">
+      <c r="G4" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/Easy-Swing-Lock-North-States/dp/B005JN6304</t>
         </is>
       </c>
-      <c r="H4" s="23" t="inlineStr">
+      <c r="H4" s="19" t="inlineStr">
         <is>
           <t>Toddleroo by North States 47.85" Wide Easy Swing &amp; Lock Baby Gate: Ideal for Wider Areas and stairways. Hardware Mount. Fits Openings 28.68" - 47.85" Wide (31" Tall, Matte Bronze)</t>
         </is>
       </c>
-      <c r="I4" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J4" s="18" t="n">
+      <c r="I4" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J4" s="16" t="n">
         <v>46.49</v>
       </c>
       <c r="K4">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L4" s="3" t="n"/>
@@ -795,25 +744,25 @@
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" s="5">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174560064792</t>
         </is>
       </c>
-      <c r="C5" s="27" t="inlineStr">
+      <c r="C5" s="19" t="inlineStr">
         <is>
           <t>Camilla Para Masajes con Cojín de Cara Tamaño Universal para Todos Sus Cliente</t>
         </is>
       </c>
-      <c r="D5" s="20" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E5" s="16" t="inlineStr">
+      <c r="D5" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E5" s="14" t="inlineStr">
         <is>
           <t>39.96</t>
         </is>
@@ -823,51 +772,51 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G5" s="22" t="inlineStr">
+      <c r="G5" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B0844RX1B7/</t>
         </is>
       </c>
-      <c r="H5" s="24" t="inlineStr">
+      <c r="H5" s="19" t="inlineStr">
         <is>
           <t>Master Massage Table Flannel Sheet Set 3 In 1 Table Cover, Face Cushion Cover, Table Sheet Black, 1count</t>
         </is>
       </c>
-      <c r="I5" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J5" s="18" t="n">
+      <c r="I5" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J5" s="16" t="n">
         <v>25.5</v>
       </c>
       <c r="K5">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L5" s="3" t="n"/>
       <c r="N5" s="3" t="n"/>
     </row>
     <row r="6" ht="18" customHeight="1" s="5">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="inlineStr">
+      <c r="B6" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174541217839</t>
         </is>
       </c>
-      <c r="C6" s="27" t="inlineStr">
+      <c r="C6" s="19" t="inlineStr">
         <is>
           <t>Crankcase Vent Filter CCV Breather Element Dodge RAM '7-'19 6.7L Diesel CV52001</t>
         </is>
       </c>
-      <c r="D6" s="20" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E6" s="16" t="inlineStr">
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E6" s="14" t="inlineStr">
         <is>
           <t>57.99</t>
         </is>
@@ -877,26 +826,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G6" s="29" t="inlineStr">
+      <c r="G6" s="20" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B08BNGPLPG</t>
         </is>
       </c>
-      <c r="H6" s="12" t="inlineStr">
+      <c r="H6" s="19" t="inlineStr">
         <is>
           <t>iFJF CV52001 Crankcase Ventilation Filter Replacement for Ram 2500 3500 4500 5500 6.7L 2007.5-2020 ISB engines Fits 904-418 4936636 68002433AC</t>
         </is>
       </c>
-      <c r="I6" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J6" s="18" t="n">
+      <c r="I6" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J6" s="16" t="n">
         <v>50</v>
       </c>
       <c r="K6">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L6" s="3" t="n"/>
@@ -911,25 +860,25 @@
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" s="5">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="inlineStr">
+      <c r="B7" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174562737540</t>
         </is>
       </c>
-      <c r="C7" s="27" t="inlineStr">
+      <c r="C7" s="19" t="inlineStr">
         <is>
           <t>Crankcase Vent Filter CCV Breather Element Dodge RAM '7-'19 6.7L Diesel CV52001</t>
         </is>
       </c>
-      <c r="D7" s="20" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E7" s="16" t="inlineStr">
+      <c r="D7" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E7" s="14" t="inlineStr">
         <is>
           <t>57.39</t>
         </is>
@@ -939,26 +888,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G7" s="22" t="inlineStr">
+      <c r="G7" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B08BNGPLPG</t>
         </is>
       </c>
-      <c r="H7" s="12" t="inlineStr">
+      <c r="H7" s="19" t="inlineStr">
         <is>
           <t>iFJF CV52001 Crankcase Ventilation Filter Replacement for Ram 2500 3500 4500 5500 6.7L 2007.5-2020 ISB engines Fits 904-418 4936636 68002433AC</t>
         </is>
       </c>
-      <c r="I7" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J7" s="18" t="n">
+      <c r="I7" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J7" s="16" t="n">
         <v>50</v>
       </c>
       <c r="K7">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L7" s="3" t="n"/>
@@ -970,25 +919,25 @@
       </c>
     </row>
     <row r="8" ht="18" customHeight="1" s="5">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="inlineStr">
+      <c r="B8" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174556048852</t>
         </is>
       </c>
-      <c r="C8" s="28" t="inlineStr">
+      <c r="C8" s="19" t="inlineStr">
         <is>
           <t>Handle Bridge Kit Table Saw Accessory Portable Push Block Wood Part Attachment</t>
         </is>
       </c>
-      <c r="D8" s="21" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E8" s="16" t="inlineStr">
+      <c r="D8" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>31.29</t>
         </is>
@@ -998,26 +947,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G8" s="13" t="inlineStr">
+      <c r="G8" s="12" t="inlineStr">
         <is>
           <t>https://www.amazon.com/GRR-RIPPER-Handle-Bridge-Kit-Accessory/dp/B0037M6J94</t>
         </is>
       </c>
-      <c r="H8" s="12" t="inlineStr">
+      <c r="H8" s="19" t="inlineStr">
         <is>
           <t>GRR-RIPPER Handle Bridge Kit (Accessory only)</t>
         </is>
       </c>
-      <c r="I8" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J8" s="18" t="n">
-        <v>14.28</v>
+      <c r="I8" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J8" s="16" t="n">
+        <v>13.88</v>
       </c>
       <c r="K8">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L8" s="3" t="n"/>
@@ -1029,25 +978,25 @@
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" s="5">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="22" t="inlineStr">
+      <c r="B9" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174526603626</t>
         </is>
       </c>
-      <c r="C9" s="27" t="inlineStr">
+      <c r="C9" s="19" t="inlineStr">
         <is>
           <t>Heavy Duty Document Shredder Industrial Page Large Paper Commercial Machine</t>
         </is>
       </c>
-      <c r="D9" s="20" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E9" s="16" t="inlineStr">
+      <c r="D9" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E9" s="14" t="inlineStr">
         <is>
           <t>50.99</t>
         </is>
@@ -1057,51 +1006,51 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G9" s="22" t="inlineStr">
+      <c r="G9" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B083XNT87B/ref=twister_B07WYL9RF8?_encoding=UTF8&amp;amp;amp;th=1</t>
         </is>
       </c>
-      <c r="H9" s="23" t="inlineStr">
+      <c r="H9" s="19" t="inlineStr">
         <is>
           <t>Aurora AU875XA Paper and Credit Card Shredder with 3.7-Gallon Wastebasket, 8-Sheet Cross-Cut with Basket</t>
         </is>
       </c>
-      <c r="I9" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J9" s="18" t="n">
+      <c r="I9" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J9" s="16" t="n">
         <v>38.93</v>
       </c>
       <c r="K9">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L9" s="3" t="n"/>
       <c r="N9" s="3" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1" s="5">
-      <c r="A10" s="14" t="n">
+      <c r="A10" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="inlineStr">
+      <c r="B10" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174542515766</t>
         </is>
       </c>
-      <c r="C10" s="28" t="inlineStr">
+      <c r="C10" s="19" t="inlineStr">
         <is>
           <t>lntex Motor Mount Kit for lntex inflatable Boats</t>
         </is>
       </c>
-      <c r="D10" s="21" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E10" s="16" t="inlineStr">
+      <c r="D10" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E10" s="14" t="inlineStr">
         <is>
           <t>74.99</t>
         </is>
@@ -1111,26 +1060,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G10" s="22" t="inlineStr">
+      <c r="G10" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/Intex-Motor-Mount-inflatable-Boats/dp/B000NNM4BW</t>
         </is>
       </c>
-      <c r="H10" s="23" t="inlineStr">
+      <c r="H10" s="19" t="inlineStr">
         <is>
           <t>Intex Motor Mount Kit for Intex inflatable Boats</t>
         </is>
       </c>
-      <c r="I10" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J10" s="18" t="n">
+      <c r="I10" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J10" s="16" t="n">
         <v>69.95999999999999</v>
       </c>
       <c r="K10">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L10" s="3" t="n"/>
@@ -1142,15 +1091,15 @@
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1" s="5">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="22" t="inlineStr">
+      <c r="B11" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174564966643</t>
         </is>
       </c>
-      <c r="C11" s="25" t="inlineStr">
+      <c r="C11" s="19" t="inlineStr">
         <is>
           <t>Pico Portable LED Mini Projector Home Cinema Theater Multi-Port Support USB HDMI</t>
         </is>
@@ -1160,7 +1109,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E11" s="16" t="inlineStr">
+      <c r="E11" s="14" t="inlineStr">
         <is>
           <t>59.99</t>
         </is>
@@ -1170,41 +1119,41 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G11" s="22" t="inlineStr">
+      <c r="G11" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/Projector-Artlii-iPhone-Pocket-Smartphone/dp/B01LYM0EY6</t>
         </is>
       </c>
-      <c r="H11" s="23" t="inlineStr">
+      <c r="H11" s="19" t="inlineStr">
         <is>
           <t>Pico Projector - Artlii 2021 New Mini Projector, Color LED Pico Projector for Cartoon, Movie, Kids Gift, Compatible with HDMI USB Laptop Video Games</t>
         </is>
       </c>
-      <c r="I11" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J11" s="18" t="n">
+      <c r="I11" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J11" s="16" t="n">
         <v>49.99</v>
       </c>
       <c r="K11">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L11" s="3" t="n"/>
       <c r="N11" s="3" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" s="5">
-      <c r="A12" s="14" t="n">
+      <c r="A12" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="inlineStr">
+      <c r="B12" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174571895207</t>
         </is>
       </c>
-      <c r="C12" s="25" t="inlineStr">
+      <c r="C12" s="19" t="inlineStr">
         <is>
           <t>Ring Chime Pro Extend Wifi Smart For Indoor Compatible with Ring App (New Model)</t>
         </is>
@@ -1214,7 +1163,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E12" s="16" t="inlineStr">
+      <c r="E12" s="14" t="inlineStr">
         <is>
           <t>56.79</t>
         </is>
@@ -1224,26 +1173,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G12" s="29" t="inlineStr">
+      <c r="G12" s="20" t="inlineStr">
         <is>
           <t>https://www.amazon.com/Ring-Chime-Pro/dp/B07WML2XTD</t>
         </is>
       </c>
-      <c r="H12" s="24" t="inlineStr">
+      <c r="H12" s="19" t="inlineStr">
         <is>
           <t>Ring Chime Pro</t>
         </is>
       </c>
-      <c r="I12" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J12" s="18" t="n">
+      <c r="I12" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J12" s="16" t="n">
         <v>49.99</v>
       </c>
       <c r="K12">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L12" s="3" t="n"/>
@@ -1255,15 +1204,15 @@
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" s="5">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="inlineStr">
+      <c r="B13" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174533135919</t>
         </is>
       </c>
-      <c r="C13" s="25" t="inlineStr">
+      <c r="C13" s="19" t="inlineStr">
         <is>
           <t>Rivet Gun Kit Rivnut Setting Tool Nut Setter 7PC NutSert Metric and amp SAE Gun</t>
         </is>
@@ -1273,7 +1222,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E13" s="16" t="inlineStr">
+      <c r="E13" s="14" t="inlineStr">
         <is>
           <t>52.99</t>
         </is>
@@ -1283,26 +1232,26 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G13" s="29" t="inlineStr">
+      <c r="G13" s="20" t="inlineStr">
         <is>
           <t>https://www.amazon.com/REXBETI-Professional-Mandrels-Labor-Saving-Carrying/dp/B07MVXN7LK/</t>
         </is>
       </c>
-      <c r="H13" s="23" t="inlineStr">
+      <c r="H13" s="19" t="inlineStr">
         <is>
           <t>REXBETI 14" Rivet Nut Tool, Professional Rivet Setter Kit with 7 Metric &amp; Sae Mandrels and 60pcs Rivnuts, Labor-Saving Design, Extra 1/4-20 mandrel with Rugged Carrying Case</t>
         </is>
       </c>
-      <c r="I13" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J13" s="18" t="n">
+      <c r="I13" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J13" s="16" t="n">
         <v>45.97</v>
       </c>
       <c r="K13">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L13" s="3" t="n"/>
@@ -1314,25 +1263,25 @@
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" s="5">
-      <c r="A14" s="14" t="n">
+      <c r="A14" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="22" t="inlineStr">
+      <c r="B14" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174571899335</t>
         </is>
       </c>
-      <c r="C14" s="26" t="inlineStr">
+      <c r="C14" s="19" t="inlineStr">
         <is>
           <t>Self Cleaning Litter Box Eco Automatic Scoopfree Pet Tray Electric Cat Waste Bin</t>
         </is>
       </c>
-      <c r="D14" s="19" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="E14" s="16" t="inlineStr">
+      <c r="D14" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="E14" s="14" t="inlineStr">
         <is>
           <t>194.99</t>
         </is>
@@ -1342,41 +1291,41 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G14" s="22" t="inlineStr">
+      <c r="G14" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B07GYX7RLD/ref=twister_B07PGW73CX?_encoding=UTF8&amp;psc=1</t>
         </is>
       </c>
-      <c r="H14" s="23" t="inlineStr">
-        <is>
-          <t>PetSafe Simply Clean Self-Cleaning Cat Litter Box, Automatic Litter Box, Works with Clumping Cat Litter</t>
-        </is>
-      </c>
-      <c r="I14" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J14" s="18" t="n">
+      <c r="H14" s="19" t="inlineStr">
+        <is>
+          <t>PetSafe Simply Clean Self Cleaning Cat Litter Box, Automatic Litter Box, Works with Clumping Cat Litter</t>
+        </is>
+      </c>
+      <c r="I14" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J14" s="16" t="n">
         <v>99.95</v>
       </c>
       <c r="K14">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L14" s="3" t="n"/>
       <c r="N14" s="3" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1" s="5">
-      <c r="A15" s="14" t="n">
+      <c r="A15" s="13" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="inlineStr">
+      <c r="B15" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174594602152</t>
         </is>
       </c>
-      <c r="C15" s="25" t="inlineStr">
+      <c r="C15" s="19" t="inlineStr">
         <is>
           <t>Set of 6 Bullnose Rubber Non-Slip Stair Treads Outdoor 30x10" Weatherproof Black</t>
         </is>
@@ -1386,7 +1335,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E15" s="16" t="inlineStr">
+      <c r="E15" s="14" t="inlineStr">
         <is>
           <t>79.99</t>
         </is>
@@ -1396,41 +1345,41 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G15" s="22" t="inlineStr">
+      <c r="G15" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/dp/B00T01O8UI</t>
         </is>
       </c>
-      <c r="H15" s="23" t="inlineStr">
+      <c r="H15" s="19" t="inlineStr">
         <is>
           <t>Rubber-Cal 6-Piece Regal Stair Treads Rubber Step Mats, 9.75 by 29.75-Inch, Black</t>
         </is>
       </c>
-      <c r="I15" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J15" s="18" t="n">
+      <c r="I15" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J15" s="16" t="n">
         <v>49.59</v>
       </c>
       <c r="K15">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L15" s="3" t="n"/>
       <c r="N15" s="3" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1" s="5">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="22" t="inlineStr">
+      <c r="B16" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174562735795</t>
         </is>
       </c>
-      <c r="C16" s="25" t="inlineStr">
+      <c r="C16" s="19" t="inlineStr">
         <is>
           <t>Dial Indicator Set Test .001 with On/Off Magneti Base Supply Magneti-c</t>
         </is>
@@ -1440,7 +1389,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E16" s="16" t="inlineStr">
+      <c r="E16" s="14" t="inlineStr">
         <is>
           <t>56.99</t>
         </is>
@@ -1450,41 +1399,41 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G16" s="22" t="inlineStr">
+      <c r="G16" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/All-Industrial-Tool-Supply-TR72020/dp/B002YPHT76</t>
         </is>
       </c>
-      <c r="H16" s="23" t="inlineStr">
+      <c r="H16" s="19" t="inlineStr">
         <is>
           <t>All Industrial Tool Supply TR72020 Dial Indicator (Magnetic Base &amp; Point Precision Inspection Set)</t>
         </is>
       </c>
-      <c r="I16" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J16" s="18" t="n">
+      <c r="I16" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J16" s="16" t="n">
         <v>37.22</v>
       </c>
       <c r="K16">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L16" s="3" t="n"/>
       <c r="N16" s="3" t="n"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" s="5">
-      <c r="A17" s="14" t="n">
+      <c r="A17" s="13" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="22" t="inlineStr">
+      <c r="B17" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174560141031</t>
         </is>
       </c>
-      <c r="C17" s="25" t="inlineStr">
+      <c r="C17" s="19" t="inlineStr">
         <is>
           <t>Stock Pot 12 Quart Aluminium Kitchen Cooker Nonstick w Glass Lid T-FaI Cookware</t>
         </is>
@@ -1494,7 +1443,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E17" s="16" t="inlineStr">
+      <c r="E17" s="14" t="inlineStr">
         <is>
           <t>84.39</t>
         </is>
@@ -1504,41 +1453,41 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G17" s="22" t="inlineStr">
+      <c r="G17" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/T-fal-Specialty-Nonstick-Dishwasher-Stockpot/dp/B000GWK34K</t>
         </is>
       </c>
-      <c r="H17" s="23" t="inlineStr">
+      <c r="H17" s="19" t="inlineStr">
         <is>
           <t>T-fal B36262 Specialty Total Nonstick Dishwasher Safe Oven Safe Stockpot Cookware, 12-Quart, Black</t>
         </is>
       </c>
-      <c r="I17" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J17" s="18" t="n">
+      <c r="I17" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J17" s="16" t="n">
         <v>39.99</v>
       </c>
       <c r="K17">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L17" s="3" t="n"/>
       <c r="N17" s="3" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1" s="5">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="13" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="22" t="inlineStr">
+      <c r="B18" s="17" t="inlineStr">
         <is>
           <t>http://www.ebay.com/itm/174549320568</t>
         </is>
       </c>
-      <c r="C18" s="25" t="inlineStr">
+      <c r="C18" s="19" t="inlineStr">
         <is>
           <t>WiIow Tree Song of Joy Angel Christmas Holiday Nativity Angel Accessory Decor</t>
         </is>
@@ -1548,7 +1497,7 @@
           <t>In Stock</t>
         </is>
       </c>
-      <c r="E18" s="16" t="inlineStr">
+      <c r="E18" s="14" t="inlineStr">
         <is>
           <t>59.99</t>
         </is>
@@ -1558,137 +1507,137 @@
           <t>derst</t>
         </is>
       </c>
-      <c r="G18" s="22" t="inlineStr">
+      <c r="G18" s="17" t="inlineStr">
         <is>
           <t>https://www.amazon.com/Demdaco-18-Inches-Willow-Tree-Angel/dp/B0071XOKGE</t>
         </is>
       </c>
-      <c r="H18" s="24" t="inlineStr">
+      <c r="H18" s="19" t="inlineStr">
         <is>
           <t>Willow Tree Song of Joy Angel, Sculpted Hand-Painted Figure</t>
         </is>
       </c>
-      <c r="I18" s="17" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-      <c r="J18" s="18" t="n">
+      <c r="I18" s="15" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="J18" s="16" t="n">
         <v>51.95</v>
       </c>
       <c r="K18">
-        <f>A2+B2+AC1</f>
+        <f>IF(E2-(E2*0.15+J2)&lt;0, TRUE, FALSE)</f>
         <v/>
       </c>
       <c r="L18" s="3" t="n"/>
       <c r="N18" s="3" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1" s="5">
-      <c r="B19" s="23" t="n"/>
-      <c r="C19" s="23" t="n"/>
-      <c r="G19" s="23" t="n"/>
-      <c r="H19" s="23" t="n"/>
+      <c r="B19" s="18" t="n"/>
+      <c r="C19" s="18" t="n"/>
+      <c r="G19" s="18" t="n"/>
+      <c r="H19" s="18" t="n"/>
     </row>
     <row r="20" ht="14.25" customHeight="1" s="5">
-      <c r="B20" s="23" t="n"/>
-      <c r="C20" s="23" t="n"/>
-      <c r="G20" s="23" t="n"/>
-      <c r="H20" s="23" t="n"/>
+      <c r="B20" s="18" t="n"/>
+      <c r="C20" s="18" t="n"/>
+      <c r="G20" s="18" t="n"/>
+      <c r="H20" s="18" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1" s="5">
-      <c r="B21" s="23" t="n"/>
-      <c r="C21" s="23" t="n"/>
-      <c r="G21" s="23" t="n"/>
-      <c r="H21" s="23" t="n"/>
+      <c r="B21" s="18" t="n"/>
+      <c r="C21" s="18" t="n"/>
+      <c r="G21" s="18" t="n"/>
+      <c r="H21" s="18" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1" s="5">
-      <c r="B22" s="23" t="n"/>
-      <c r="C22" s="23" t="n"/>
-      <c r="G22" s="23" t="n"/>
-      <c r="H22" s="23" t="n"/>
+      <c r="B22" s="18" t="n"/>
+      <c r="C22" s="18" t="n"/>
+      <c r="G22" s="18" t="n"/>
+      <c r="H22" s="18" t="n"/>
     </row>
     <row r="23" ht="14.25" customHeight="1" s="5">
-      <c r="B23" s="23" t="n"/>
-      <c r="C23" s="23" t="n"/>
-      <c r="G23" s="23" t="n"/>
-      <c r="H23" s="23" t="n"/>
+      <c r="B23" s="18" t="n"/>
+      <c r="C23" s="18" t="n"/>
+      <c r="G23" s="18" t="n"/>
+      <c r="H23" s="18" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1" s="5">
-      <c r="B24" s="23" t="n"/>
-      <c r="C24" s="23" t="n"/>
-      <c r="G24" s="23" t="n"/>
-      <c r="H24" s="23" t="n"/>
+      <c r="B24" s="18" t="n"/>
+      <c r="C24" s="18" t="n"/>
+      <c r="G24" s="18" t="n"/>
+      <c r="H24" s="18" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1" s="5">
-      <c r="B25" s="23" t="n"/>
-      <c r="C25" s="23" t="n"/>
-      <c r="G25" s="23" t="n"/>
-      <c r="H25" s="23" t="n"/>
+      <c r="B25" s="18" t="n"/>
+      <c r="C25" s="18" t="n"/>
+      <c r="G25" s="18" t="n"/>
+      <c r="H25" s="18" t="n"/>
     </row>
     <row r="26" ht="14.25" customHeight="1" s="5">
-      <c r="B26" s="23" t="n"/>
-      <c r="C26" s="23" t="n"/>
-      <c r="G26" s="23" t="n"/>
-      <c r="H26" s="23" t="n"/>
+      <c r="B26" s="18" t="n"/>
+      <c r="C26" s="18" t="n"/>
+      <c r="G26" s="18" t="n"/>
+      <c r="H26" s="18" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1" s="5">
-      <c r="B27" s="23" t="n"/>
-      <c r="C27" s="23" t="n"/>
-      <c r="G27" s="23" t="n"/>
-      <c r="H27" s="23" t="n"/>
+      <c r="B27" s="18" t="n"/>
+      <c r="C27" s="18" t="n"/>
+      <c r="G27" s="18" t="n"/>
+      <c r="H27" s="18" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1" s="5">
-      <c r="B28" s="23" t="n"/>
-      <c r="C28" s="23" t="n"/>
-      <c r="G28" s="23" t="n"/>
-      <c r="H28" s="23" t="n"/>
+      <c r="B28" s="18" t="n"/>
+      <c r="C28" s="18" t="n"/>
+      <c r="G28" s="18" t="n"/>
+      <c r="H28" s="18" t="n"/>
     </row>
     <row r="29" ht="14.25" customHeight="1" s="5">
-      <c r="B29" s="23" t="n"/>
-      <c r="C29" s="23" t="n"/>
-      <c r="G29" s="23" t="n"/>
-      <c r="H29" s="23" t="n"/>
+      <c r="B29" s="18" t="n"/>
+      <c r="C29" s="18" t="n"/>
+      <c r="G29" s="18" t="n"/>
+      <c r="H29" s="18" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1" s="5">
-      <c r="B30" s="23" t="n"/>
-      <c r="C30" s="23" t="n"/>
-      <c r="G30" s="23" t="n"/>
-      <c r="H30" s="23" t="n"/>
+      <c r="B30" s="18" t="n"/>
+      <c r="C30" s="18" t="n"/>
+      <c r="G30" s="18" t="n"/>
+      <c r="H30" s="18" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" s="5">
-      <c r="B31" s="23" t="n"/>
-      <c r="C31" s="23" t="n"/>
-      <c r="G31" s="23" t="n"/>
-      <c r="H31" s="23" t="n"/>
+      <c r="B31" s="18" t="n"/>
+      <c r="C31" s="18" t="n"/>
+      <c r="G31" s="18" t="n"/>
+      <c r="H31" s="18" t="n"/>
     </row>
     <row r="32" ht="14.25" customHeight="1" s="5">
-      <c r="C32" s="23" t="n"/>
-      <c r="G32" s="23" t="n"/>
-      <c r="H32" s="23" t="n"/>
+      <c r="C32" s="18" t="n"/>
+      <c r="G32" s="18" t="n"/>
+      <c r="H32" s="18" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1" s="5">
-      <c r="C33" s="23" t="n"/>
-      <c r="G33" s="23" t="n"/>
-      <c r="H33" s="23" t="n"/>
+      <c r="C33" s="18" t="n"/>
+      <c r="G33" s="18" t="n"/>
+      <c r="H33" s="18" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1" s="5">
-      <c r="C34" s="23" t="n"/>
-      <c r="G34" s="23" t="n"/>
-      <c r="H34" s="23" t="n"/>
+      <c r="C34" s="18" t="n"/>
+      <c r="G34" s="18" t="n"/>
+      <c r="H34" s="18" t="n"/>
     </row>
     <row r="35" ht="14.25" customHeight="1" s="5">
-      <c r="C35" s="23" t="n"/>
-      <c r="G35" s="23" t="n"/>
-      <c r="H35" s="23" t="n"/>
+      <c r="C35" s="18" t="n"/>
+      <c r="G35" s="18" t="n"/>
+      <c r="H35" s="18" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1" s="5">
-      <c r="C36" s="23" t="n"/>
+      <c r="C36" s="18" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1" s="5">
-      <c r="C37" s="23" t="n"/>
+      <c r="C37" s="18" t="n"/>
     </row>
     <row r="38" ht="14.25" customHeight="1" s="5">
-      <c r="C38" s="23" t="n"/>
+      <c r="C38" s="18" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1" s="5"/>
     <row r="40" ht="14.25" customHeight="1" s="5"/>

</xml_diff>